<commit_message>
fetch words from excel and map it to object
</commit_message>
<xml_diff>
--- a/assets/languages.xlsx
+++ b/assets/languages.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t>English</t>
   </si>
@@ -44,22 +44,181 @@
     <t>italian</t>
   </si>
   <si>
-    <t xml:space="preserve">Hello </t>
-  </si>
-  <si>
-    <t>salut</t>
-  </si>
-  <si>
-    <t>marhaba</t>
-  </si>
-  <si>
-    <t>dqd</t>
-  </si>
-  <si>
-    <t>Hola</t>
-  </si>
-  <si>
-    <t>Sq</t>
+    <t>JOUER</t>
+  </si>
+  <si>
+    <t>NIVEAU</t>
+  </si>
+  <si>
+    <t>MODE DEFI</t>
+  </si>
+  <si>
+    <t>Conneciox facebook</t>
+  </si>
+  <si>
+    <t>AMATEUR</t>
+  </si>
+  <si>
+    <t>EXPERT</t>
+  </si>
+  <si>
+    <t>QUITTER</t>
+  </si>
+  <si>
+    <t>MON RECORD</t>
+  </si>
+  <si>
+    <t>Connected vous pour decouvrir votre classement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAY </t>
+  </si>
+  <si>
+    <t>لعب</t>
+  </si>
+  <si>
+    <t>JUGAR</t>
+  </si>
+  <si>
+    <t>TONEELSTUK</t>
+  </si>
+  <si>
+    <t>GIOCARE</t>
+  </si>
+  <si>
+    <t>LEVEL</t>
+  </si>
+  <si>
+    <t>مستوى</t>
+  </si>
+  <si>
+    <t>NIVEL</t>
+  </si>
+  <si>
+    <t>LIVELLO</t>
+  </si>
+  <si>
+    <t>CHALLENGE MODE</t>
+  </si>
+  <si>
+    <t>وضع التحدي</t>
+  </si>
+  <si>
+    <t>UITDAGINGSMODUS</t>
+  </si>
+  <si>
+    <t>MODO DESAFÍO</t>
+  </si>
+  <si>
+    <t>MODALITÀ SFIDA</t>
+  </si>
+  <si>
+    <t>Facebook login</t>
+  </si>
+  <si>
+    <t>تسجيل الدخول الى الفيسبوك</t>
+  </si>
+  <si>
+    <t>Facebook-login</t>
+  </si>
+  <si>
+    <t>Inicio de sesión en Facebook</t>
+  </si>
+  <si>
+    <t>Accesso a Facebook</t>
+  </si>
+  <si>
+    <t>DÉBUTANT</t>
+  </si>
+  <si>
+    <t>BEGINNER</t>
+  </si>
+  <si>
+    <t>مبتدئ</t>
+  </si>
+  <si>
+    <t>PRINCIPIANTE</t>
+  </si>
+  <si>
+    <t>AFICIONADA</t>
+  </si>
+  <si>
+    <t>AMATORIALE</t>
+  </si>
+  <si>
+    <t>الهواة</t>
+  </si>
+  <si>
+    <t>خبير</t>
+  </si>
+  <si>
+    <t>DESKUNDIGE</t>
+  </si>
+  <si>
+    <t>EXPERTO</t>
+  </si>
+  <si>
+    <t>ESPERTO</t>
+  </si>
+  <si>
+    <t>AVERTI</t>
+  </si>
+  <si>
+    <t>INFORMED</t>
+  </si>
+  <si>
+    <t>مطلع</t>
+  </si>
+  <si>
+    <t>OP DE HOOGTE</t>
+  </si>
+  <si>
+    <t>INFORMADA</t>
+  </si>
+  <si>
+    <t>INFORMATA</t>
+  </si>
+  <si>
+    <t>LEAVE</t>
+  </si>
+  <si>
+    <t>غادر</t>
+  </si>
+  <si>
+    <t>VERTREKKEN</t>
+  </si>
+  <si>
+    <t>SALIR</t>
+  </si>
+  <si>
+    <t>PARTIRE</t>
+  </si>
+  <si>
+    <t>MY RECORD</t>
+  </si>
+  <si>
+    <t>السجل الخاص بي</t>
+  </si>
+  <si>
+    <t>MIJN REGISTRATIE</t>
+  </si>
+  <si>
+    <t>MI REGISTRO</t>
+  </si>
+  <si>
+    <t>IL MIO DOCUMENTO</t>
+  </si>
+  <si>
+    <t>Log in to find out your ranking</t>
+  </si>
+  <si>
+    <t>تسجيل الدخول لمعرفة الترتيب الخاص بك</t>
+  </si>
+  <si>
+    <t>Log in om je ranking te zien</t>
+  </si>
+  <si>
+    <t>Inicie sesión para conocer su clasificación</t>
   </si>
 </sst>
 </file>
@@ -377,13 +536,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -407,22 +573,222 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add dependcies to user facebook login
</commit_message>
<xml_diff>
--- a/assets/languages.xlsx
+++ b/assets/languages.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <t>English</t>
   </si>
@@ -219,6 +219,24 @@
   </si>
   <si>
     <t>Inicie sesión para conocer su clasificación</t>
+  </si>
+  <si>
+    <t>DEFI</t>
+  </si>
+  <si>
+    <t>CHALLENGE</t>
+  </si>
+  <si>
+    <t>تحد</t>
+  </si>
+  <si>
+    <t>UITDAGING</t>
+  </si>
+  <si>
+    <t>DESAFÍO</t>
+  </si>
+  <si>
+    <t>SFIDA</t>
   </si>
 </sst>
 </file>
@@ -536,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,6 +809,26 @@
         <v>64</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add sending personal best functionality
</commit_message>
<xml_diff>
--- a/assets/languages.xlsx
+++ b/assets/languages.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="112">
   <si>
     <t>English</t>
   </si>
@@ -237,6 +237,129 @@
   </si>
   <si>
     <t>SFIDA</t>
+  </si>
+  <si>
+    <t>facebook friends ranking</t>
+  </si>
+  <si>
+    <t>classement amis facebook</t>
+  </si>
+  <si>
+    <t>ترتيب أصدقاء الفيسبوك</t>
+  </si>
+  <si>
+    <t>classifica amici di facebook</t>
+  </si>
+  <si>
+    <t>Facebook vrienden ranking</t>
+  </si>
+  <si>
+    <t>Ranking de amigos de facebook</t>
+  </si>
+  <si>
+    <t>pas le temps</t>
+  </si>
+  <si>
+    <t>لا وقت</t>
+  </si>
+  <si>
+    <t>geen tijd</t>
+  </si>
+  <si>
+    <t>no hay tiempo</t>
+  </si>
+  <si>
+    <t>non c'è tempo</t>
+  </si>
+  <si>
+    <t>Felicidades Ganas con Récord de</t>
+  </si>
+  <si>
+    <t>Congratulation You Win with Record of</t>
+  </si>
+  <si>
+    <t>Félicitation vous gagnez avec enregistrement de</t>
+  </si>
+  <si>
+    <t>Congratulazioni hai vinto con record di</t>
+  </si>
+  <si>
+    <t>Gefeliciteerd, je wint met een record van</t>
+  </si>
+  <si>
+    <t>مبروك فوزك بسجل</t>
+  </si>
+  <si>
+    <t>يتم استهلاك جميع العمليات حاول مرة أخرى</t>
+  </si>
+  <si>
+    <t>toutes les opérations sont consommées réessayez</t>
+  </si>
+  <si>
+    <t>todas las operaciones se han consumido inténtalo de nuevo</t>
+  </si>
+  <si>
+    <t>alle bewerkingen zijn verbruikt probeer het opnieuw</t>
+  </si>
+  <si>
+    <t>tutte le operazioni sono state consumate riprovare</t>
+  </si>
+  <si>
+    <t>all operation are consumed try again</t>
+  </si>
+  <si>
+    <t>Tu as perdu</t>
+  </si>
+  <si>
+    <t>You Lost</t>
+  </si>
+  <si>
+    <t>Perdiste</t>
+  </si>
+  <si>
+    <t>لقد خسرت</t>
+  </si>
+  <si>
+    <t>je hebt verloren</t>
+  </si>
+  <si>
+    <t>Hai perso</t>
+  </si>
+  <si>
+    <t>خلف</t>
+  </si>
+  <si>
+    <t>Arrière</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Rug</t>
+  </si>
+  <si>
+    <t>Atrás</t>
+  </si>
+  <si>
+    <t>Di ritorno</t>
+  </si>
+  <si>
+    <t>Ops ottieni un valore decimale riprova</t>
+  </si>
+  <si>
+    <t>Ops you get decimal value try again</t>
+  </si>
+  <si>
+    <t>Ops تحصل على قيمة عشرية حاول مرة أخرى</t>
+  </si>
+  <si>
+    <t>Oeps, je krijgt een decimale waarde, probeer het opnieuw</t>
+  </si>
+  <si>
+    <t>Ops, obtienes un valor decimal, inténtalo de nuevo</t>
+  </si>
+  <si>
+    <t>No Time</t>
   </si>
 </sst>
 </file>
@@ -554,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -829,6 +952,143 @@
         <v>70</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F20" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>